<commit_message>
updated excel file data of registration
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kadahari\Desktop\Harika\C\Demoblaze\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF6B795-7D89-4229-97E3-90CD6A95F7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D6F101-7DC9-4AA2-929B-D967897D82CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6195" yWindow="1800" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{C530B214-C532-48CA-9507-3FBA420147F2}"/>
+    <workbookView xWindow="6540" yWindow="2145" windowWidth="21600" windowHeight="11295" xr2:uid="{C530B214-C532-48CA-9507-3FBA420147F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>validPass123</t>
   </si>
@@ -223,10 +223,13 @@
     <t>ValidPass@23</t>
   </si>
   <si>
-    <t>Validuser223</t>
-  </si>
-  <si>
     <t>MultipleAdd</t>
+  </si>
+  <si>
+    <t>Validuser45</t>
+  </si>
+  <si>
+    <t>ValidPass@45</t>
   </si>
 </sst>
 </file>
@@ -285,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -313,6 +316,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9BB8137-2EE2-4733-BA03-EA3CA42D19B0}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,10 +661,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>14</v>
@@ -938,7 +942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEB0BA2A-7A13-430D-A737-AC7B0C214942}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -1039,7 +1043,7 @@
         <v>36</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="7">
         <v>2</v>

</xml_diff>